<commit_message>
Encryption and folders implemented
</commit_message>
<xml_diff>
--- a/Lucas Wu.xlsx
+++ b/Lucas Wu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="146">
   <si>
     <t>Eduardo da Costa</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Karolyna G. Schenk</t>
   </si>
   <si>
-    <t>Larissa Oliveira</t>
-  </si>
-  <si>
     <t>Luca Crepaldi</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
     <t>Bruno Ukoski</t>
   </si>
   <si>
+    <t>Eduardo Marins</t>
+  </si>
+  <si>
     <t>Fran Dároitt</t>
   </si>
   <si>
@@ -149,6 +149,9 @@
     <t>Kleber Coelho</t>
   </si>
   <si>
+    <t>Paula Fuks</t>
+  </si>
+  <si>
     <t>Co-Founder &amp; COO</t>
   </si>
   <si>
@@ -179,9 +182,6 @@
     <t>M&amp;A and Corporate Development Executive Director at TOTVS | Chief M&amp;A and Corporate Development Officer | Technology</t>
   </si>
   <si>
-    <t>Senior Software Engineer</t>
-  </si>
-  <si>
     <t>M&amp;A at Cypress</t>
   </si>
   <si>
@@ -191,7 +191,7 @@
     <t>Founder at Agrosmart | Bloomberg most influential in Latam | Forbes under 30 | MIT TR35 | Fast Company Most Creative | ESG | Digital Farming | Future of Food</t>
   </si>
   <si>
-    <t>Safra Digital</t>
+    <t>Diretor Digital, Financeira e Cartões</t>
   </si>
   <si>
     <t>Head of Americas Facilities Operations Management</t>
@@ -245,6 +245,9 @@
     <t>CTO &amp; Co-Founder na Agidesk</t>
   </si>
   <si>
+    <t>Operations Intern at Sistema B</t>
+  </si>
+  <si>
     <t>Co-Founder</t>
   </si>
   <si>
@@ -257,7 +260,7 @@
     <t>Partner at Crescera Capital</t>
   </si>
   <si>
-    <t>CEO na TALLOS | MindShifter 2021 | Especialista em vendas Omnichannel |</t>
+    <t>CEO na TALLOS | MindShifter 2021 | Vendas Omnichannel | Scale Up Endeavor | Growth hacking</t>
   </si>
   <si>
     <t>Co-Founder at madamecrème</t>
@@ -278,6 +281,9 @@
     <t>CEO - BEMBRAS Defense &amp; Security</t>
   </si>
   <si>
+    <t>Diretora de Admissão na Innovation Experience Israel</t>
+  </si>
+  <si>
     <t>https://www.linkedin.com/in/edu-da-costa-carvalho/</t>
   </si>
   <si>
@@ -308,9 +314,6 @@
     <t>https://www.linkedin.com/in/karolynaguedes</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/larrrrcr</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/lucacrepaldi</t>
   </si>
   <si>
@@ -377,6 +380,9 @@
     <t>https://www.linkedin.com/in/brunoukoski</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/eduardoafmarins</t>
+  </si>
+  <si>
     <t>https://www.linkedin.com/in/frandaroitt/</t>
   </si>
   <si>
@@ -408,6 +414,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/klebercoelhojunior</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/paula-fuks-082842121</t>
   </si>
   <si>
     <t>Nome</t>
@@ -831,7 +840,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B6:E50"/>
+  <dimension ref="B6:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -843,16 +852,16 @@
   <sheetData>
     <row r="6" spans="2:5">
       <c r="B6" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:5" s="2" customFormat="1">
@@ -860,10 +869,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="2:5" s="4" customFormat="1">
@@ -871,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:5" s="4" customFormat="1">
@@ -882,10 +891,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="2:5" s="4" customFormat="1">
@@ -893,10 +902,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="2:5" s="4" customFormat="1">
@@ -904,10 +913,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:5" s="4" customFormat="1">
@@ -915,10 +924,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="2:5" s="4" customFormat="1">
@@ -926,10 +935,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="2:5" s="4" customFormat="1">
@@ -937,10 +946,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="2:5" s="4" customFormat="1">
@@ -948,10 +957,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="2:5" s="4" customFormat="1">
@@ -959,10 +968,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="2:4" s="4" customFormat="1">
@@ -970,10 +979,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="2:4" s="4" customFormat="1">
@@ -981,10 +990,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:4" s="4" customFormat="1">
@@ -992,10 +1001,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="2:4" s="4" customFormat="1">
@@ -1003,10 +1012,10 @@
         <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="2:4" s="4" customFormat="1">
@@ -1014,10 +1023,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="2:4" s="4" customFormat="1">
@@ -1025,10 +1034,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:4" s="4" customFormat="1">
@@ -1036,10 +1045,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:4" s="4" customFormat="1">
@@ -1047,10 +1056,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:4" s="4" customFormat="1">
@@ -1058,10 +1067,10 @@
         <v>18</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:4" s="4" customFormat="1">
@@ -1069,32 +1078,32 @@
         <v>19</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" s="4" customFormat="1">
-      <c r="B27" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" s="2" customFormat="1">
+      <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>64</v>
+      <c r="C27" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" s="2" customFormat="1">
-      <c r="B28" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" s="4" customFormat="1">
+      <c r="B28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>65</v>
+      <c r="C28" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="2:4" s="4" customFormat="1">
@@ -1102,32 +1111,32 @@
         <v>22</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" s="4" customFormat="1">
-      <c r="B30" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" s="2" customFormat="1">
+      <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>67</v>
+      <c r="C30" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" s="2" customFormat="1">
-      <c r="B31" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" s="4" customFormat="1">
+      <c r="B31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>68</v>
+      <c r="C31" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:4" s="4" customFormat="1">
@@ -1135,10 +1144,10 @@
         <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:4" s="4" customFormat="1">
@@ -1146,10 +1155,10 @@
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="2:4" s="4" customFormat="1">
@@ -1157,10 +1166,10 @@
         <v>27</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="2:4" s="4" customFormat="1">
@@ -1168,10 +1177,10 @@
         <v>28</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="2:4" s="4" customFormat="1">
@@ -1179,32 +1188,32 @@
         <v>29</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" s="4" customFormat="1">
-      <c r="B37" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" s="2" customFormat="1">
+      <c r="B37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>74</v>
+      <c r="C37" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" s="2" customFormat="1">
-      <c r="B38" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" s="4" customFormat="1">
+      <c r="B38" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>65</v>
+      <c r="C38" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="2:4" s="4" customFormat="1">
@@ -1212,10 +1221,10 @@
         <v>32</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="2:4" s="2" customFormat="1">
@@ -1223,10 +1232,10 @@
         <v>33</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="2:4" s="4" customFormat="1">
@@ -1234,10 +1243,10 @@
         <v>34</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="2:4" s="2" customFormat="1">
@@ -1245,10 +1254,10 @@
         <v>35</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="2:4" s="4" customFormat="1">
@@ -1256,10 +1265,10 @@
         <v>36</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="2:4" s="4" customFormat="1">
@@ -1267,10 +1276,10 @@
         <v>37</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="2:4" s="4" customFormat="1">
@@ -1278,10 +1287,10 @@
         <v>38</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="2:4" s="4" customFormat="1">
@@ -1289,10 +1298,10 @@
         <v>39</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="2:4" s="4" customFormat="1">
@@ -1300,10 +1309,10 @@
         <v>40</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="2:4" s="2" customFormat="1">
@@ -1311,10 +1320,10 @@
         <v>41</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="2:4" s="4" customFormat="1">
@@ -1322,10 +1331,10 @@
         <v>42</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="2:4" s="4" customFormat="1">
@@ -1333,10 +1342,21 @@
         <v>43</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" s="4" customFormat="1">
+      <c r="B51" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1385,6 +1405,7 @@
     <hyperlink ref="D48" r:id="rId42"/>
     <hyperlink ref="D49" r:id="rId43"/>
     <hyperlink ref="D50" r:id="rId44"/>
+    <hyperlink ref="D51" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1392,7 +1413,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1400,1155 +1421,1086 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>65</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>65</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F27" t="s">
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
         <v>68</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F34" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G35" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G36" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G37" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
         <v>35</v>
       </c>
       <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" t="s">
-        <v>37</v>
-      </c>
-      <c r="G38" t="s">
-        <v>80</v>
-      </c>
       <c r="H38" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="G39" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F40" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G40" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
         <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="G42" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G44" t="s">
-        <v>83</v>
-      </c>
       <c r="H44" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
         <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G45" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B46" t="s">
         <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F46" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="G46" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F47" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F48" t="s">
-        <v>43</v>
-      </c>
-      <c r="G48" t="s">
-        <v>86</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F49" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" t="s">
-        <v>54</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" t="s">
-        <v>142</v>
-      </c>
-      <c r="B50" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" t="s">
-        <v>55</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2646,12 +2598,6 @@
     <hyperlink ref="H46" r:id="rId90"/>
     <hyperlink ref="D47" r:id="rId91"/>
     <hyperlink ref="H47" r:id="rId92"/>
-    <hyperlink ref="D48" r:id="rId93"/>
-    <hyperlink ref="H48" r:id="rId94"/>
-    <hyperlink ref="D49" r:id="rId95"/>
-    <hyperlink ref="H49" r:id="rId96"/>
-    <hyperlink ref="D50" r:id="rId97"/>
-    <hyperlink ref="H50" r:id="rId98"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>